<commit_message>
fix server and html
</commit_message>
<xml_diff>
--- a/server/file/block/宿舍楼模板.xlsx
+++ b/server/file/block/宿舍楼模板.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6189DD8-ADDA-4C26-A943-2E2EF509AAC2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F722DE1-B0D7-49EE-8ED4-5C2520469770}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,10 +36,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3号楼-男</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>宿舍大小（几人间）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -52,10 +48,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4号楼-女</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>性别</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -65,6 +57,14 @@
   </si>
   <si>
     <t>女</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9号楼-男</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10号楼-女</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -393,7 +393,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -410,13 +410,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -424,7 +424,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>6</v>
@@ -433,7 +433,7 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -441,7 +441,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -450,7 +450,7 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -475,10 +475,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1052,10 +1052,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>